<commit_message>
Update cours du matin
</commit_message>
<xml_diff>
--- a/Exos/04-tp-complet/01-tp-video-club/01-tp-video-club.xlsx
+++ b/Exos/04-tp-complet/01-tp-video-club/01-tp-video-club.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\REPO-GITHUB\CDA-07-DB\Exos\04-tp-complet\01-tp-video-club\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA140551-57FD-4A3D-8642-1B6DEC7F9574}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6635AF6-8C42-4BB5-BD0C-53E499A8F98B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="17640" xr2:uid="{CFFC525C-6FE4-4BAF-972D-B3DFB1CD5250}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{CFFC525C-6FE4-4BAF-972D-B3DFB1CD5250}"/>
   </bookViews>
   <sheets>
     <sheet name="Dictionnaire de données" sheetId="1" r:id="rId1"/>
     <sheet name="Matrice vanilla" sheetId="2" r:id="rId2"/>
-    <sheet name="Dépendances fonctionnelles simp" sheetId="3" r:id="rId3"/>
+    <sheet name="Dépendances fonctionnelles simp" sheetId="5" r:id="rId3"/>
+    <sheet name="Dépendances fonctionnelles comp" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="73">
   <si>
     <t>Mnemonique</t>
   </si>
@@ -242,13 +243,25 @@
   </si>
   <si>
     <t>Nom de la rue</t>
+  </si>
+  <si>
+    <t>(movie_title, movie_director)</t>
+  </si>
+  <si>
+    <t>(actor_name, actor_firstname, actor_birth)</t>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
+    <t>→</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -271,8 +284,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -327,8 +348,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -377,49 +410,77 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -429,6 +490,87 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -743,10 +885,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AF74A7F-FA35-438F-A0F3-6FB00DD605E2}">
-  <dimension ref="B4:H30"/>
+  <dimension ref="B4:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -760,368 +902,371 @@
     <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="6" t="s">
+    <row r="4" spans="2:12" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="6" t="s">
+      <c r="C4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-    </row>
-    <row r="5" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="8" t="s">
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="L4">
+        <v>2147483648</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="5">
         <v>10</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-    </row>
-    <row r="6" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="8" t="s">
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+    </row>
+    <row r="6" spans="2:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="5">
         <v>50</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-    </row>
-    <row r="7" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="8" t="s">
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+    </row>
+    <row r="7" spans="2:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="5">
         <v>50</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-    </row>
-    <row r="8" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="8" t="s">
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+    </row>
+    <row r="8" spans="2:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="26"/>
-      <c r="H8" s="27"/>
-    </row>
-    <row r="9" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="8" t="s">
+      <c r="G8" s="23"/>
+      <c r="H8" s="24"/>
+    </row>
+    <row r="9" spans="2:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="5">
         <v>3</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-    </row>
-    <row r="10" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="17" t="s">
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+    </row>
+    <row r="10" spans="2:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10" s="9">
         <v>10</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="F10" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-    </row>
-    <row r="11" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="17" t="s">
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+    </row>
+    <row r="11" spans="2:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="17">
+      <c r="E11" s="9">
         <v>50</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-    </row>
-    <row r="12" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="17" t="s">
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+    </row>
+    <row r="12" spans="2:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="17">
+      <c r="E12" s="9">
         <v>50</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="F12" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="24"/>
-      <c r="H12" s="25"/>
-    </row>
-    <row r="13" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="19" t="s">
+      <c r="G12" s="30"/>
+      <c r="H12" s="31"/>
+    </row>
+    <row r="13" spans="2:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="19">
+      <c r="E13" s="10">
         <v>50</v>
       </c>
-      <c r="F13" s="19" t="s">
+      <c r="F13" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-    </row>
-    <row r="14" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="19" t="s">
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+    </row>
+    <row r="14" spans="2:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="19">
+      <c r="E14" s="10">
         <v>100</v>
       </c>
-      <c r="F14" s="19" t="s">
+      <c r="F14" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-    </row>
-    <row r="15" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="19" t="s">
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+    </row>
+    <row r="15" spans="2:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="19">
+      <c r="E15" s="10">
         <v>5</v>
       </c>
-      <c r="F15" s="19" t="s">
+      <c r="F15" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G15" s="21" t="s">
+      <c r="G15" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="H15" s="21"/>
-    </row>
-    <row r="16" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="22" t="s">
+      <c r="H15" s="28"/>
+    </row>
+    <row r="16" spans="2:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="22" t="s">
+      <c r="D16" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="22">
+      <c r="E16" s="11">
         <v>50</v>
       </c>
-      <c r="F16" s="22" t="s">
+      <c r="F16" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
     </row>
     <row r="17" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="22" t="s">
+      <c r="D17" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E17" s="22">
+      <c r="E17" s="11">
         <v>50</v>
       </c>
-      <c r="F17" s="22" t="s">
+      <c r="F17" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
     </row>
     <row r="18" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="22" t="s">
+      <c r="C18" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="22" t="s">
+      <c r="D18" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="22" t="s">
+      <c r="E18" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="F18" s="22" t="s">
+      <c r="F18" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="G18" s="23"/>
-      <c r="H18" s="23"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
     </row>
     <row r="19" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="22" t="s">
+      <c r="C19" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="22" t="s">
+      <c r="D19" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="22">
+      <c r="E19" s="11">
         <v>20</v>
       </c>
-      <c r="F19" s="22" t="s">
+      <c r="F19" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G19" s="23"/>
-      <c r="H19" s="23"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
     </row>
     <row r="20" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="10">
+      <c r="E20" s="6">
         <v>10</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="F20" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G20" s="11"/>
-      <c r="H20" s="12"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="26"/>
     </row>
     <row r="21" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G21" s="11"/>
-      <c r="H21" s="12"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="26"/>
     </row>
     <row r="22" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E22" s="10">
+      <c r="E22" s="6">
         <v>50</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="F22" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G22" s="11"/>
-      <c r="H22" s="12"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="26"/>
     </row>
     <row r="23" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
@@ -1139,10 +1284,10 @@
       <c r="F23" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="G23" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="H23" s="5"/>
+      <c r="H23" s="20"/>
     </row>
     <row r="24" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
@@ -1160,132 +1305,136 @@
       <c r="F24" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G24" s="4" t="s">
+      <c r="G24" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="H24" s="5"/>
+      <c r="H24" s="20"/>
     </row>
     <row r="25" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D25" s="13" t="s">
+      <c r="D25" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E25" s="13">
+      <c r="E25" s="7">
         <v>50</v>
       </c>
-      <c r="F25" s="14" t="s">
+      <c r="F25" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G25" s="15"/>
-      <c r="H25" s="16"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="18"/>
     </row>
     <row r="26" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="28" t="s">
+      <c r="B26" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="C26" s="28" t="s">
+      <c r="C26" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="D26" s="28" t="s">
+      <c r="D26" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E26" s="28">
+      <c r="E26" s="12">
         <v>10</v>
       </c>
-      <c r="F26" s="29" t="s">
+      <c r="F26" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="G26" s="31"/>
-      <c r="H26" s="32"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="16"/>
     </row>
     <row r="27" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="28" t="s">
+      <c r="B27" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="C27" s="28" t="s">
+      <c r="C27" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="D27" s="28" t="s">
+      <c r="D27" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E27" s="28">
+      <c r="E27" s="12">
         <v>5</v>
       </c>
-      <c r="F27" s="28" t="s">
+      <c r="F27" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="G27" s="30"/>
-      <c r="H27" s="30"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
     </row>
     <row r="28" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="28" t="s">
+      <c r="B28" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="C28" s="28" t="s">
+      <c r="C28" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="D28" s="28" t="s">
+      <c r="D28" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E28" s="28">
+      <c r="E28" s="12">
         <v>50</v>
       </c>
-      <c r="F28" s="28" t="s">
+      <c r="F28" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="G28" s="30"/>
-      <c r="H28" s="30"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
     </row>
     <row r="29" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="28" t="s">
+      <c r="B29" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="C29" s="28" t="s">
+      <c r="C29" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="D29" s="28" t="s">
+      <c r="D29" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E29" s="28">
+      <c r="E29" s="12">
         <v>10</v>
       </c>
-      <c r="F29" s="28" t="s">
+      <c r="F29" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G29" s="30"/>
-      <c r="H29" s="30"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
     </row>
     <row r="30" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="28" t="s">
+      <c r="B30" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="C30" s="28" t="s">
+      <c r="C30" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="D30" s="28" t="s">
+      <c r="D30" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E30" s="28">
+      <c r="E30" s="12">
         <v>100</v>
       </c>
-      <c r="F30" s="28" t="s">
+      <c r="F30" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="G30" s="30"/>
-      <c r="H30" s="30"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G12:H12"/>
     <mergeCell ref="G25:H25"/>
     <mergeCell ref="G23:H23"/>
     <mergeCell ref="G24:H24"/>
@@ -1299,15 +1448,11 @@
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="G18:H18"/>
     <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G26:H26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1316,28 +1461,1767 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9473B4C0-DC07-794D-836D-FCE9B2D5E845}">
-  <dimension ref="A1"/>
+  <dimension ref="B3:L30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L30" sqref="B4:L30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" style="33"/>
+    <col min="2" max="2" width="20.28515625" style="35" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="33" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" style="33" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" style="33" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" style="33" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" style="33" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5703125" style="33" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" style="33" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5703125" style="33" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" style="33" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="33" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="11.42578125" style="33"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:12" s="34" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="36"/>
+      <c r="C4" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="L4" s="37" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="37"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="37"/>
+    </row>
+    <row r="6" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="37">
+        <v>1</v>
+      </c>
+      <c r="D6" s="37"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="47"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="37"/>
+    </row>
+    <row r="7" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="37">
+        <v>1</v>
+      </c>
+      <c r="D7" s="37"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="47"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="37"/>
+    </row>
+    <row r="8" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="37">
+        <v>1</v>
+      </c>
+      <c r="D8" s="37"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="47"/>
+      <c r="J8" s="37"/>
+      <c r="K8" s="37"/>
+      <c r="L8" s="37"/>
+    </row>
+    <row r="9" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="37">
+        <v>1</v>
+      </c>
+      <c r="D9" s="37"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="47"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="37"/>
+      <c r="L9" s="37"/>
+    </row>
+    <row r="10" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="43">
+        <v>1</v>
+      </c>
+      <c r="F10" s="43"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="50"/>
+      <c r="J10" s="42"/>
+      <c r="K10" s="42"/>
+      <c r="L10" s="42"/>
+    </row>
+    <row r="11" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42">
+        <v>1</v>
+      </c>
+      <c r="E11" s="43">
+        <v>1</v>
+      </c>
+      <c r="F11" s="43"/>
+      <c r="G11" s="48"/>
+      <c r="H11" s="49"/>
+      <c r="I11" s="50"/>
+      <c r="J11" s="42"/>
+      <c r="K11" s="42"/>
+      <c r="L11" s="42"/>
+    </row>
+    <row r="12" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42">
+        <v>1</v>
+      </c>
+      <c r="E12" s="43">
+        <v>1</v>
+      </c>
+      <c r="F12" s="43"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="50"/>
+      <c r="J12" s="42"/>
+      <c r="K12" s="42"/>
+      <c r="L12" s="42"/>
+    </row>
+    <row r="13" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="39" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="40">
+        <v>1</v>
+      </c>
+      <c r="F13" s="40"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="46"/>
+      <c r="I13" s="47"/>
+      <c r="J13" s="37"/>
+      <c r="K13" s="37"/>
+      <c r="L13" s="37"/>
+    </row>
+    <row r="14" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="40">
+        <v>1</v>
+      </c>
+      <c r="F14" s="40"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="46"/>
+      <c r="I14" s="47"/>
+      <c r="J14" s="37"/>
+      <c r="K14" s="37"/>
+      <c r="L14" s="37"/>
+    </row>
+    <row r="15" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="40">
+        <v>1</v>
+      </c>
+      <c r="F15" s="40"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="46"/>
+      <c r="I15" s="47"/>
+      <c r="J15" s="37"/>
+      <c r="K15" s="37"/>
+      <c r="L15" s="37"/>
+    </row>
+    <row r="16" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="48">
+        <v>1</v>
+      </c>
+      <c r="H16" s="49"/>
+      <c r="I16" s="50"/>
+      <c r="J16" s="42"/>
+      <c r="K16" s="42"/>
+      <c r="L16" s="42"/>
+    </row>
+    <row r="17" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="48">
+        <v>1</v>
+      </c>
+      <c r="H17" s="49"/>
+      <c r="I17" s="50"/>
+      <c r="J17" s="42"/>
+      <c r="K17" s="42"/>
+      <c r="L17" s="42"/>
+    </row>
+    <row r="18" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="48">
+        <v>1</v>
+      </c>
+      <c r="H18" s="49"/>
+      <c r="I18" s="50"/>
+      <c r="J18" s="42"/>
+      <c r="K18" s="42"/>
+      <c r="L18" s="42"/>
+    </row>
+    <row r="19" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="48">
+        <v>1</v>
+      </c>
+      <c r="H19" s="49"/>
+      <c r="I19" s="50"/>
+      <c r="J19" s="42"/>
+      <c r="K19" s="42"/>
+      <c r="L19" s="42"/>
+    </row>
+    <row r="20" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="45"/>
+      <c r="H20" s="46"/>
+      <c r="I20" s="47"/>
+      <c r="J20" s="37"/>
+      <c r="K20" s="37"/>
+      <c r="L20" s="37"/>
+    </row>
+    <row r="21" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="45"/>
+      <c r="H21" s="46"/>
+      <c r="I21" s="47"/>
+      <c r="J21" s="37">
+        <v>1</v>
+      </c>
+      <c r="K21" s="37"/>
+      <c r="L21" s="37"/>
+    </row>
+    <row r="22" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="37"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="45"/>
+      <c r="H22" s="46"/>
+      <c r="I22" s="47"/>
+      <c r="J22" s="37">
+        <v>1</v>
+      </c>
+      <c r="K22" s="37"/>
+      <c r="L22" s="37"/>
+    </row>
+    <row r="23" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="44" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" s="42"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="48"/>
+      <c r="H23" s="49"/>
+      <c r="I23" s="50"/>
+      <c r="J23" s="42"/>
+      <c r="K23" s="42"/>
+      <c r="L23" s="42"/>
+    </row>
+    <row r="24" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="44" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" s="42"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="48"/>
+      <c r="H24" s="49"/>
+      <c r="I24" s="50"/>
+      <c r="J24" s="42"/>
+      <c r="K24" s="42"/>
+      <c r="L24" s="42"/>
+    </row>
+    <row r="25" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="45"/>
+      <c r="H25" s="46"/>
+      <c r="I25" s="47"/>
+      <c r="J25" s="37"/>
+      <c r="K25" s="37"/>
+      <c r="L25" s="37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="C26" s="42">
+        <v>1</v>
+      </c>
+      <c r="D26" s="42"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="43"/>
+      <c r="G26" s="48"/>
+      <c r="H26" s="49"/>
+      <c r="I26" s="50"/>
+      <c r="J26" s="42"/>
+      <c r="K26" s="42">
+        <v>1</v>
+      </c>
+      <c r="L26" s="42"/>
+    </row>
+    <row r="27" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="44" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" s="42">
+        <v>1</v>
+      </c>
+      <c r="D27" s="42"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="43"/>
+      <c r="G27" s="48"/>
+      <c r="H27" s="49"/>
+      <c r="I27" s="50"/>
+      <c r="J27" s="42"/>
+      <c r="K27" s="42">
+        <v>1</v>
+      </c>
+      <c r="L27" s="42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="44" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" s="42">
+        <v>1</v>
+      </c>
+      <c r="D28" s="42"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="48"/>
+      <c r="H28" s="49"/>
+      <c r="I28" s="50"/>
+      <c r="J28" s="42"/>
+      <c r="K28" s="42">
+        <v>1</v>
+      </c>
+      <c r="L28" s="42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="42">
+        <v>1</v>
+      </c>
+      <c r="D29" s="42"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="48"/>
+      <c r="H29" s="49"/>
+      <c r="I29" s="50"/>
+      <c r="J29" s="42"/>
+      <c r="K29" s="42">
+        <v>1</v>
+      </c>
+      <c r="L29" s="42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="44" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" s="42">
+        <v>1</v>
+      </c>
+      <c r="D30" s="42"/>
+      <c r="E30" s="43"/>
+      <c r="F30" s="43"/>
+      <c r="G30" s="48"/>
+      <c r="H30" s="49"/>
+      <c r="I30" s="50"/>
+      <c r="J30" s="42"/>
+      <c r="K30" s="42">
+        <v>1</v>
+      </c>
+      <c r="L30" s="42">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="52">
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C8D2C94-6DDA-5441-ADE7-C625043D60DD}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43F70A41-356E-4DCE-81CF-AD1213A03A07}">
+  <dimension ref="B7:Y30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10:X16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="1.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="1.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="1.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="1.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="21.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="7" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="36"/>
+      <c r="C8" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="J8" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="L8" s="37" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="37">
+        <v>1</v>
+      </c>
+      <c r="D9" s="37"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="47"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="37"/>
+      <c r="L9" s="37"/>
+    </row>
+    <row r="10" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="37">
+        <v>1</v>
+      </c>
+      <c r="D10" s="37"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="47"/>
+      <c r="J10" s="37"/>
+      <c r="K10" s="37"/>
+      <c r="L10" s="37"/>
+      <c r="N10" s="52" t="s">
+        <v>13</v>
+      </c>
+      <c r="O10" s="52" t="s">
+        <v>72</v>
+      </c>
+      <c r="P10" s="53" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q10" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="R10" s="53" t="s">
+        <v>15</v>
+      </c>
+      <c r="S10" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="T10" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="U10" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="V10" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="W10" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="X10" s="53" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y10" s="51"/>
+    </row>
+    <row r="11" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="37">
+        <v>1</v>
+      </c>
+      <c r="D11" s="37"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="47"/>
+      <c r="J11" s="37"/>
+      <c r="K11" s="37"/>
+      <c r="L11" s="37"/>
+      <c r="N11" s="52" t="s">
+        <v>52</v>
+      </c>
+      <c r="O11" s="52" t="s">
+        <v>72</v>
+      </c>
+      <c r="P11" s="53" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q11" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="R11" s="53" t="s">
+        <v>54</v>
+      </c>
+      <c r="S11" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="T11" s="53"/>
+      <c r="U11" s="53"/>
+      <c r="V11" s="53"/>
+      <c r="W11" s="53"/>
+      <c r="X11" s="53"/>
+      <c r="Y11" s="51"/>
+    </row>
+    <row r="12" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="37">
+        <v>1</v>
+      </c>
+      <c r="D12" s="37"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="45"/>
+      <c r="H12" s="46"/>
+      <c r="I12" s="47"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="37"/>
+      <c r="L12" s="37"/>
+      <c r="N12" s="52" t="s">
+        <v>69</v>
+      </c>
+      <c r="O12" s="52" t="s">
+        <v>72</v>
+      </c>
+      <c r="P12" s="53" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q12" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="R12" s="53" t="s">
+        <v>24</v>
+      </c>
+      <c r="S12" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="T12" s="53" t="s">
+        <v>25</v>
+      </c>
+      <c r="U12" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="V12" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="W12" s="53"/>
+      <c r="X12" s="53"/>
+      <c r="Y12" s="51"/>
+    </row>
+    <row r="13" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="42"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="43">
+        <v>1</v>
+      </c>
+      <c r="F13" s="43"/>
+      <c r="G13" s="48"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="50"/>
+      <c r="J13" s="42"/>
+      <c r="K13" s="42"/>
+      <c r="L13" s="42"/>
+      <c r="N13" s="52" t="s">
+        <v>70</v>
+      </c>
+      <c r="O13" s="52" t="s">
+        <v>72</v>
+      </c>
+      <c r="P13" s="53" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q13" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="R13" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="S13" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="T13" s="53" t="s">
+        <v>34</v>
+      </c>
+      <c r="U13" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="V13" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="W13" s="53"/>
+      <c r="X13" s="53"/>
+      <c r="Y13" s="51"/>
+    </row>
+    <row r="14" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="42"/>
+      <c r="D14" s="42">
+        <v>1</v>
+      </c>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="48"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="50"/>
+      <c r="J14" s="42"/>
+      <c r="K14" s="42"/>
+      <c r="L14" s="42"/>
+      <c r="N14" s="52" t="s">
+        <v>23</v>
+      </c>
+      <c r="O14" s="52" t="s">
+        <v>72</v>
+      </c>
+      <c r="P14" s="53" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q14" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="R14" s="53" t="s">
+        <v>43</v>
+      </c>
+      <c r="S14" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="T14" s="53"/>
+      <c r="U14" s="53"/>
+      <c r="V14" s="53"/>
+      <c r="W14" s="53"/>
+      <c r="X14" s="53"/>
+      <c r="Y14" s="51"/>
+    </row>
+    <row r="15" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="42"/>
+      <c r="D15" s="42">
+        <v>1</v>
+      </c>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="48"/>
+      <c r="H15" s="49"/>
+      <c r="I15" s="50"/>
+      <c r="J15" s="42"/>
+      <c r="K15" s="42"/>
+      <c r="L15" s="42"/>
+      <c r="N15" s="52" t="s">
+        <v>49</v>
+      </c>
+      <c r="O15" s="52" t="s">
+        <v>72</v>
+      </c>
+      <c r="P15" s="53" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q15" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="R15" s="53"/>
+      <c r="S15" s="53"/>
+      <c r="T15" s="53"/>
+      <c r="U15" s="53"/>
+      <c r="V15" s="53"/>
+      <c r="W15" s="53"/>
+      <c r="X15" s="53"/>
+      <c r="Y15" s="51"/>
+    </row>
+    <row r="16" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="39" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="40">
+        <v>1</v>
+      </c>
+      <c r="F16" s="40"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="46"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="37"/>
+      <c r="K16" s="37"/>
+      <c r="L16" s="37"/>
+      <c r="N16" s="52" t="s">
+        <v>65</v>
+      </c>
+      <c r="O16" s="52" t="s">
+        <v>72</v>
+      </c>
+      <c r="P16" s="53" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q16" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="R16" s="53" t="s">
+        <v>59</v>
+      </c>
+      <c r="S16" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="T16" s="53" t="s">
+        <v>60</v>
+      </c>
+      <c r="U16" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="V16" s="53" t="s">
+        <v>61</v>
+      </c>
+      <c r="W16" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="X16" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y16" s="51"/>
+    </row>
+    <row r="17" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="40">
+        <v>1</v>
+      </c>
+      <c r="F17" s="40"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="37"/>
+      <c r="K17" s="37"/>
+      <c r="L17" s="37"/>
+    </row>
+    <row r="18" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="40">
+        <v>1</v>
+      </c>
+      <c r="F18" s="40"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="37"/>
+      <c r="K18" s="37"/>
+      <c r="L18" s="37"/>
+    </row>
+    <row r="19" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="48">
+        <v>1</v>
+      </c>
+      <c r="H19" s="49"/>
+      <c r="I19" s="50"/>
+      <c r="J19" s="42"/>
+      <c r="K19" s="42"/>
+      <c r="L19" s="42"/>
+    </row>
+    <row r="20" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="42"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="48">
+        <v>1</v>
+      </c>
+      <c r="H20" s="49"/>
+      <c r="I20" s="50"/>
+      <c r="J20" s="42"/>
+      <c r="K20" s="42"/>
+      <c r="L20" s="42"/>
+    </row>
+    <row r="21" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="42"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="48">
+        <v>1</v>
+      </c>
+      <c r="H21" s="49"/>
+      <c r="I21" s="50"/>
+      <c r="J21" s="42"/>
+      <c r="K21" s="42"/>
+      <c r="L21" s="42"/>
+    </row>
+    <row r="22" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="42"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="43"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="48">
+        <v>1</v>
+      </c>
+      <c r="H22" s="49"/>
+      <c r="I22" s="50"/>
+      <c r="J22" s="42"/>
+      <c r="K22" s="42"/>
+      <c r="L22" s="42"/>
+    </row>
+    <row r="23" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="46"/>
+      <c r="I23" s="47"/>
+      <c r="J23" s="37">
+        <v>1</v>
+      </c>
+      <c r="K23" s="37"/>
+      <c r="L23" s="37"/>
+    </row>
+    <row r="24" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="37"/>
+      <c r="D24" s="37"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="45"/>
+      <c r="H24" s="46"/>
+      <c r="I24" s="47"/>
+      <c r="J24" s="37">
+        <v>1</v>
+      </c>
+      <c r="K24" s="37"/>
+      <c r="L24" s="37"/>
+    </row>
+    <row r="25" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="45"/>
+      <c r="H25" s="46"/>
+      <c r="I25" s="47"/>
+      <c r="J25" s="37"/>
+      <c r="K25" s="37"/>
+      <c r="L25" s="37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="C26" s="42">
+        <v>1</v>
+      </c>
+      <c r="D26" s="42"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="43"/>
+      <c r="G26" s="48"/>
+      <c r="H26" s="49"/>
+      <c r="I26" s="50"/>
+      <c r="J26" s="42"/>
+      <c r="K26" s="42">
+        <v>1</v>
+      </c>
+      <c r="L26" s="42"/>
+    </row>
+    <row r="27" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="44" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="43"/>
+      <c r="G27" s="48"/>
+      <c r="H27" s="49"/>
+      <c r="I27" s="50"/>
+      <c r="J27" s="42"/>
+      <c r="K27" s="42"/>
+      <c r="L27" s="42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="44" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" s="42"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="48"/>
+      <c r="H28" s="49"/>
+      <c r="I28" s="50"/>
+      <c r="J28" s="42"/>
+      <c r="K28" s="42"/>
+      <c r="L28" s="42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="42"/>
+      <c r="D29" s="42"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="48"/>
+      <c r="H29" s="49"/>
+      <c r="I29" s="50"/>
+      <c r="J29" s="42"/>
+      <c r="K29" s="42"/>
+      <c r="L29" s="42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="44" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" s="42"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="43"/>
+      <c r="F30" s="43"/>
+      <c r="G30" s="48"/>
+      <c r="H30" s="49"/>
+      <c r="I30" s="50"/>
+      <c r="J30" s="42"/>
+      <c r="K30" s="42"/>
+      <c r="L30" s="42">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="44">
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:I11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C8D2C94-6DDA-5441-ADE7-C625043D60DD}">
+  <dimension ref="D7:N30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="7" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D8" s="36"/>
+      <c r="E8" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="J8" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="K8" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="L8" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="M8" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="N8" s="37" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D9" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="37">
+        <v>1</v>
+      </c>
+      <c r="F9" s="37"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="45"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="47"/>
+      <c r="L9" s="37"/>
+      <c r="M9" s="37"/>
+      <c r="N9" s="37"/>
+    </row>
+    <row r="10" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D10" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="37">
+        <v>1</v>
+      </c>
+      <c r="F10" s="37"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="45"/>
+      <c r="J10" s="46"/>
+      <c r="K10" s="47"/>
+      <c r="L10" s="37"/>
+      <c r="M10" s="37"/>
+      <c r="N10" s="37"/>
+    </row>
+    <row r="11" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D11" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="37">
+        <v>1</v>
+      </c>
+      <c r="F11" s="37"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="45"/>
+      <c r="J11" s="46"/>
+      <c r="K11" s="47"/>
+      <c r="L11" s="37"/>
+      <c r="M11" s="37"/>
+      <c r="N11" s="37"/>
+    </row>
+    <row r="12" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D12" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="37">
+        <v>1</v>
+      </c>
+      <c r="F12" s="37"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="45"/>
+      <c r="J12" s="46"/>
+      <c r="K12" s="47"/>
+      <c r="L12" s="37"/>
+      <c r="M12" s="37"/>
+      <c r="N12" s="37"/>
+    </row>
+    <row r="13" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D13" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="43">
+        <v>1</v>
+      </c>
+      <c r="H13" s="43"/>
+      <c r="I13" s="48"/>
+      <c r="J13" s="49"/>
+      <c r="K13" s="50"/>
+      <c r="L13" s="42"/>
+      <c r="M13" s="42"/>
+      <c r="N13" s="42"/>
+    </row>
+    <row r="14" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D14" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42">
+        <v>1</v>
+      </c>
+      <c r="G14" s="43">
+        <v>1</v>
+      </c>
+      <c r="H14" s="43"/>
+      <c r="I14" s="48"/>
+      <c r="J14" s="49"/>
+      <c r="K14" s="50"/>
+      <c r="L14" s="42"/>
+      <c r="M14" s="42"/>
+      <c r="N14" s="42"/>
+    </row>
+    <row r="15" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D15" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="42"/>
+      <c r="F15" s="42">
+        <v>1</v>
+      </c>
+      <c r="G15" s="43">
+        <v>1</v>
+      </c>
+      <c r="H15" s="43"/>
+      <c r="I15" s="48"/>
+      <c r="J15" s="49"/>
+      <c r="K15" s="50"/>
+      <c r="L15" s="42"/>
+      <c r="M15" s="42"/>
+      <c r="N15" s="42"/>
+    </row>
+    <row r="16" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D16" s="39" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="40">
+        <v>1</v>
+      </c>
+      <c r="H16" s="40"/>
+      <c r="I16" s="45"/>
+      <c r="J16" s="46"/>
+      <c r="K16" s="47"/>
+      <c r="L16" s="37"/>
+      <c r="M16" s="37"/>
+      <c r="N16" s="37"/>
+    </row>
+    <row r="17" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D17" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="40">
+        <v>1</v>
+      </c>
+      <c r="H17" s="40"/>
+      <c r="I17" s="45"/>
+      <c r="J17" s="46"/>
+      <c r="K17" s="47"/>
+      <c r="L17" s="37"/>
+      <c r="M17" s="37"/>
+      <c r="N17" s="37"/>
+    </row>
+    <row r="18" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D18" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="37"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="40">
+        <v>1</v>
+      </c>
+      <c r="H18" s="40"/>
+      <c r="I18" s="45"/>
+      <c r="J18" s="46"/>
+      <c r="K18" s="47"/>
+      <c r="L18" s="37"/>
+      <c r="M18" s="37"/>
+      <c r="N18" s="37"/>
+    </row>
+    <row r="19" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D19" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
+      <c r="G19" s="43"/>
+      <c r="H19" s="43"/>
+      <c r="I19" s="48">
+        <v>1</v>
+      </c>
+      <c r="J19" s="49"/>
+      <c r="K19" s="50"/>
+      <c r="L19" s="42"/>
+      <c r="M19" s="42"/>
+      <c r="N19" s="42"/>
+    </row>
+    <row r="20" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D20" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" s="42"/>
+      <c r="F20" s="42"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="48">
+        <v>1</v>
+      </c>
+      <c r="J20" s="49"/>
+      <c r="K20" s="50"/>
+      <c r="L20" s="42"/>
+      <c r="M20" s="42"/>
+      <c r="N20" s="42"/>
+    </row>
+    <row r="21" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D21" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" s="42"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="43"/>
+      <c r="I21" s="48">
+        <v>1</v>
+      </c>
+      <c r="J21" s="49"/>
+      <c r="K21" s="50"/>
+      <c r="L21" s="42"/>
+      <c r="M21" s="42"/>
+      <c r="N21" s="42"/>
+    </row>
+    <row r="22" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D22" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="E22" s="42"/>
+      <c r="F22" s="42"/>
+      <c r="G22" s="43"/>
+      <c r="H22" s="43"/>
+      <c r="I22" s="48">
+        <v>1</v>
+      </c>
+      <c r="J22" s="49"/>
+      <c r="K22" s="50"/>
+      <c r="L22" s="42"/>
+      <c r="M22" s="42"/>
+      <c r="N22" s="42"/>
+    </row>
+    <row r="23" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D23" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="E23" s="37"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="45"/>
+      <c r="J23" s="46"/>
+      <c r="K23" s="47"/>
+      <c r="L23" s="37">
+        <v>1</v>
+      </c>
+      <c r="M23" s="37"/>
+      <c r="N23" s="37"/>
+    </row>
+    <row r="24" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D24" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" s="37"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="45"/>
+      <c r="J24" s="46"/>
+      <c r="K24" s="47"/>
+      <c r="L24" s="37">
+        <v>1</v>
+      </c>
+      <c r="M24" s="37"/>
+      <c r="N24" s="37"/>
+    </row>
+    <row r="25" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D25" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="E25" s="37"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="40"/>
+      <c r="H25" s="40"/>
+      <c r="I25" s="45"/>
+      <c r="J25" s="46"/>
+      <c r="K25" s="47"/>
+      <c r="L25" s="37"/>
+      <c r="M25" s="37"/>
+      <c r="N25" s="37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D26" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="E26" s="42">
+        <v>1</v>
+      </c>
+      <c r="F26" s="42"/>
+      <c r="G26" s="43"/>
+      <c r="H26" s="43"/>
+      <c r="I26" s="48"/>
+      <c r="J26" s="49"/>
+      <c r="K26" s="50"/>
+      <c r="L26" s="42"/>
+      <c r="M26" s="42">
+        <v>1</v>
+      </c>
+      <c r="N26" s="42"/>
+    </row>
+    <row r="27" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D27" s="44" t="s">
+        <v>59</v>
+      </c>
+      <c r="E27" s="42">
+        <v>1</v>
+      </c>
+      <c r="F27" s="42"/>
+      <c r="G27" s="43"/>
+      <c r="H27" s="43"/>
+      <c r="I27" s="48"/>
+      <c r="J27" s="49"/>
+      <c r="K27" s="50"/>
+      <c r="L27" s="42"/>
+      <c r="M27" s="42">
+        <v>1</v>
+      </c>
+      <c r="N27" s="42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D28" s="44" t="s">
+        <v>60</v>
+      </c>
+      <c r="E28" s="42">
+        <v>1</v>
+      </c>
+      <c r="F28" s="42"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="48"/>
+      <c r="J28" s="49"/>
+      <c r="K28" s="50"/>
+      <c r="L28" s="42"/>
+      <c r="M28" s="42">
+        <v>1</v>
+      </c>
+      <c r="N28" s="42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D29" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="E29" s="42">
+        <v>1</v>
+      </c>
+      <c r="F29" s="42"/>
+      <c r="G29" s="43"/>
+      <c r="H29" s="43"/>
+      <c r="I29" s="48"/>
+      <c r="J29" s="49"/>
+      <c r="K29" s="50"/>
+      <c r="L29" s="42"/>
+      <c r="M29" s="42">
+        <v>1</v>
+      </c>
+      <c r="N29" s="42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D30" s="44" t="s">
+        <v>62</v>
+      </c>
+      <c r="E30" s="42">
+        <v>1</v>
+      </c>
+      <c r="F30" s="42"/>
+      <c r="G30" s="43"/>
+      <c r="H30" s="43"/>
+      <c r="I30" s="48"/>
+      <c r="J30" s="49"/>
+      <c r="K30" s="50"/>
+      <c r="L30" s="42"/>
+      <c r="M30" s="42">
+        <v>1</v>
+      </c>
+      <c r="N30" s="42">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="44">
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="I29:K29"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="I30:K30"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="I27:K27"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:K28"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="I25:K25"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="I13:K13"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:K10"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Commimt des fichiers modifies
</commit_message>
<xml_diff>
--- a/Exos/04-tp-complet/01-tp-video-club/01-tp-video-club.xlsx
+++ b/Exos/04-tp-complet/01-tp-video-club/01-tp-video-club.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\REPO-GITHUB\CDA-07-DB\Exos\04-tp-complet\01-tp-video-club\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6635AF6-8C42-4BB5-BD0C-53E499A8F98B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54CC790E-76FE-4F01-95B5-BB3FABC63E70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{CFFC525C-6FE4-4BAF-972D-B3DFB1CD5250}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{CFFC525C-6FE4-4BAF-972D-B3DFB1CD5250}"/>
   </bookViews>
   <sheets>
     <sheet name="Dictionnaire de données" sheetId="1" r:id="rId1"/>
     <sheet name="Matrice vanilla" sheetId="2" r:id="rId2"/>
     <sheet name="Dépendances fonctionnelles simp" sheetId="5" r:id="rId3"/>
-    <sheet name="Dépendances fonctionnelles comp" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="73">
   <si>
     <t>Mnemonique</t>
   </si>
@@ -885,9 +884,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AF74A7F-FA35-438F-A0F3-6FB00DD605E2}">
-  <dimension ref="B4:L30"/>
+  <dimension ref="B4:H30"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
@@ -902,7 +901,7 @@
     <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:12" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>0</v>
       </c>
@@ -920,11 +919,8 @@
       </c>
       <c r="G4" s="32"/>
       <c r="H4" s="32"/>
-      <c r="L4">
-        <v>2147483648</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>13</v>
       </c>
@@ -943,7 +939,7 @@
       <c r="G5" s="21"/>
       <c r="H5" s="21"/>
     </row>
-    <row r="6" spans="2:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>14</v>
       </c>
@@ -962,7 +958,7 @@
       <c r="G6" s="21"/>
       <c r="H6" s="21"/>
     </row>
-    <row r="7" spans="2:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>15</v>
       </c>
@@ -981,7 +977,7 @@
       <c r="G7" s="21"/>
       <c r="H7" s="21"/>
     </row>
-    <row r="8" spans="2:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>21</v>
       </c>
@@ -1000,7 +996,7 @@
       <c r="G8" s="23"/>
       <c r="H8" s="24"/>
     </row>
-    <row r="9" spans="2:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>16</v>
       </c>
@@ -1019,7 +1015,7 @@
       <c r="G9" s="21"/>
       <c r="H9" s="21"/>
     </row>
-    <row r="10" spans="2:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="9" t="s">
         <v>52</v>
       </c>
@@ -1038,7 +1034,7 @@
       <c r="G10" s="22"/>
       <c r="H10" s="22"/>
     </row>
-    <row r="11" spans="2:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="s">
         <v>53</v>
       </c>
@@ -1057,7 +1053,7 @@
       <c r="G11" s="22"/>
       <c r="H11" s="22"/>
     </row>
-    <row r="12" spans="2:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="9" t="s">
         <v>54</v>
       </c>
@@ -1076,7 +1072,7 @@
       <c r="G12" s="30"/>
       <c r="H12" s="31"/>
     </row>
-    <row r="13" spans="2:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="10" t="s">
         <v>24</v>
       </c>
@@ -1095,7 +1091,7 @@
       <c r="G13" s="29"/>
       <c r="H13" s="29"/>
     </row>
-    <row r="14" spans="2:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="10" t="s">
         <v>25</v>
       </c>
@@ -1114,7 +1110,7 @@
       <c r="G14" s="29"/>
       <c r="H14" s="29"/>
     </row>
-    <row r="15" spans="2:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="10" t="s">
         <v>26</v>
       </c>
@@ -1135,7 +1131,7 @@
       </c>
       <c r="H15" s="28"/>
     </row>
-    <row r="16" spans="2:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="11" t="s">
         <v>32</v>
       </c>
@@ -1464,7 +1460,7 @@
   <dimension ref="B3:L30"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L30" sqref="B4:L30"/>
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2037,8 +2033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43F70A41-356E-4DCE-81CF-AD1213A03A07}">
   <dimension ref="B7:Y30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10:X16"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2369,9 +2365,7 @@
       <c r="P15" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="Q15" s="53" t="s">
-        <v>71</v>
-      </c>
+      <c r="Q15" s="53"/>
       <c r="R15" s="53"/>
       <c r="S15" s="53"/>
       <c r="T15" s="53"/>
@@ -2721,507 +2715,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C8D2C94-6DDA-5441-ADE7-C625043D60DD}">
-  <dimension ref="D7:N30"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="7" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D8" s="36"/>
-      <c r="E8" s="37" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="37" t="s">
-        <v>52</v>
-      </c>
-      <c r="G8" s="38" t="s">
-        <v>24</v>
-      </c>
-      <c r="H8" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="I8" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="J8" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="K8" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="L8" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="M8" s="37" t="s">
-        <v>49</v>
-      </c>
-      <c r="N8" s="37" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="9" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D9" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="37">
-        <v>1</v>
-      </c>
-      <c r="F9" s="37"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="45"/>
-      <c r="J9" s="46"/>
-      <c r="K9" s="47"/>
-      <c r="L9" s="37"/>
-      <c r="M9" s="37"/>
-      <c r="N9" s="37"/>
-    </row>
-    <row r="10" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D10" s="36" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="37">
-        <v>1</v>
-      </c>
-      <c r="F10" s="37"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="45"/>
-      <c r="J10" s="46"/>
-      <c r="K10" s="47"/>
-      <c r="L10" s="37"/>
-      <c r="M10" s="37"/>
-      <c r="N10" s="37"/>
-    </row>
-    <row r="11" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D11" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="37">
-        <v>1</v>
-      </c>
-      <c r="F11" s="37"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="45"/>
-      <c r="J11" s="46"/>
-      <c r="K11" s="47"/>
-      <c r="L11" s="37"/>
-      <c r="M11" s="37"/>
-      <c r="N11" s="37"/>
-    </row>
-    <row r="12" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D12" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="37">
-        <v>1</v>
-      </c>
-      <c r="F12" s="37"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="45"/>
-      <c r="J12" s="46"/>
-      <c r="K12" s="47"/>
-      <c r="L12" s="37"/>
-      <c r="M12" s="37"/>
-      <c r="N12" s="37"/>
-    </row>
-    <row r="13" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D13" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="E13" s="42"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="43">
-        <v>1</v>
-      </c>
-      <c r="H13" s="43"/>
-      <c r="I13" s="48"/>
-      <c r="J13" s="49"/>
-      <c r="K13" s="50"/>
-      <c r="L13" s="42"/>
-      <c r="M13" s="42"/>
-      <c r="N13" s="42"/>
-    </row>
-    <row r="14" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="E14" s="42"/>
-      <c r="F14" s="42">
-        <v>1</v>
-      </c>
-      <c r="G14" s="43">
-        <v>1</v>
-      </c>
-      <c r="H14" s="43"/>
-      <c r="I14" s="48"/>
-      <c r="J14" s="49"/>
-      <c r="K14" s="50"/>
-      <c r="L14" s="42"/>
-      <c r="M14" s="42"/>
-      <c r="N14" s="42"/>
-    </row>
-    <row r="15" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D15" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42">
-        <v>1</v>
-      </c>
-      <c r="G15" s="43">
-        <v>1</v>
-      </c>
-      <c r="H15" s="43"/>
-      <c r="I15" s="48"/>
-      <c r="J15" s="49"/>
-      <c r="K15" s="50"/>
-      <c r="L15" s="42"/>
-      <c r="M15" s="42"/>
-      <c r="N15" s="42"/>
-    </row>
-    <row r="16" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D16" s="39" t="s">
-        <v>24</v>
-      </c>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="40">
-        <v>1</v>
-      </c>
-      <c r="H16" s="40"/>
-      <c r="I16" s="45"/>
-      <c r="J16" s="46"/>
-      <c r="K16" s="47"/>
-      <c r="L16" s="37"/>
-      <c r="M16" s="37"/>
-      <c r="N16" s="37"/>
-    </row>
-    <row r="17" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D17" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="E17" s="37"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="40">
-        <v>1</v>
-      </c>
-      <c r="H17" s="40"/>
-      <c r="I17" s="45"/>
-      <c r="J17" s="46"/>
-      <c r="K17" s="47"/>
-      <c r="L17" s="37"/>
-      <c r="M17" s="37"/>
-      <c r="N17" s="37"/>
-    </row>
-    <row r="18" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D18" s="36" t="s">
-        <v>26</v>
-      </c>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="40">
-        <v>1</v>
-      </c>
-      <c r="H18" s="40"/>
-      <c r="I18" s="45"/>
-      <c r="J18" s="46"/>
-      <c r="K18" s="47"/>
-      <c r="L18" s="37"/>
-      <c r="M18" s="37"/>
-      <c r="N18" s="37"/>
-    </row>
-    <row r="19" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D19" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="E19" s="42"/>
-      <c r="F19" s="42"/>
-      <c r="G19" s="43"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="48">
-        <v>1</v>
-      </c>
-      <c r="J19" s="49"/>
-      <c r="K19" s="50"/>
-      <c r="L19" s="42"/>
-      <c r="M19" s="42"/>
-      <c r="N19" s="42"/>
-    </row>
-    <row r="20" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D20" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="E20" s="42"/>
-      <c r="F20" s="42"/>
-      <c r="G20" s="43"/>
-      <c r="H20" s="43"/>
-      <c r="I20" s="48">
-        <v>1</v>
-      </c>
-      <c r="J20" s="49"/>
-      <c r="K20" s="50"/>
-      <c r="L20" s="42"/>
-      <c r="M20" s="42"/>
-      <c r="N20" s="42"/>
-    </row>
-    <row r="21" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D21" s="41" t="s">
-        <v>34</v>
-      </c>
-      <c r="E21" s="42"/>
-      <c r="F21" s="42"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="43"/>
-      <c r="I21" s="48">
-        <v>1</v>
-      </c>
-      <c r="J21" s="49"/>
-      <c r="K21" s="50"/>
-      <c r="L21" s="42"/>
-      <c r="M21" s="42"/>
-      <c r="N21" s="42"/>
-    </row>
-    <row r="22" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D22" s="44" t="s">
-        <v>35</v>
-      </c>
-      <c r="E22" s="42"/>
-      <c r="F22" s="42"/>
-      <c r="G22" s="43"/>
-      <c r="H22" s="43"/>
-      <c r="I22" s="48">
-        <v>1</v>
-      </c>
-      <c r="J22" s="49"/>
-      <c r="K22" s="50"/>
-      <c r="L22" s="42"/>
-      <c r="M22" s="42"/>
-      <c r="N22" s="42"/>
-    </row>
-    <row r="23" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D23" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="E23" s="37"/>
-      <c r="F23" s="37"/>
-      <c r="G23" s="40"/>
-      <c r="H23" s="40"/>
-      <c r="I23" s="45"/>
-      <c r="J23" s="46"/>
-      <c r="K23" s="47"/>
-      <c r="L23" s="37">
-        <v>1</v>
-      </c>
-      <c r="M23" s="37"/>
-      <c r="N23" s="37"/>
-    </row>
-    <row r="24" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D24" s="36" t="s">
-        <v>43</v>
-      </c>
-      <c r="E24" s="37"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="45"/>
-      <c r="J24" s="46"/>
-      <c r="K24" s="47"/>
-      <c r="L24" s="37">
-        <v>1</v>
-      </c>
-      <c r="M24" s="37"/>
-      <c r="N24" s="37"/>
-    </row>
-    <row r="25" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D25" s="39" t="s">
-        <v>49</v>
-      </c>
-      <c r="E25" s="37"/>
-      <c r="F25" s="37"/>
-      <c r="G25" s="40"/>
-      <c r="H25" s="40"/>
-      <c r="I25" s="45"/>
-      <c r="J25" s="46"/>
-      <c r="K25" s="47"/>
-      <c r="L25" s="37"/>
-      <c r="M25" s="37"/>
-      <c r="N25" s="37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D26" s="41" t="s">
-        <v>65</v>
-      </c>
-      <c r="E26" s="42">
-        <v>1</v>
-      </c>
-      <c r="F26" s="42"/>
-      <c r="G26" s="43"/>
-      <c r="H26" s="43"/>
-      <c r="I26" s="48"/>
-      <c r="J26" s="49"/>
-      <c r="K26" s="50"/>
-      <c r="L26" s="42"/>
-      <c r="M26" s="42">
-        <v>1</v>
-      </c>
-      <c r="N26" s="42"/>
-    </row>
-    <row r="27" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D27" s="44" t="s">
-        <v>59</v>
-      </c>
-      <c r="E27" s="42">
-        <v>1</v>
-      </c>
-      <c r="F27" s="42"/>
-      <c r="G27" s="43"/>
-      <c r="H27" s="43"/>
-      <c r="I27" s="48"/>
-      <c r="J27" s="49"/>
-      <c r="K27" s="50"/>
-      <c r="L27" s="42"/>
-      <c r="M27" s="42">
-        <v>1</v>
-      </c>
-      <c r="N27" s="42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D28" s="44" t="s">
-        <v>60</v>
-      </c>
-      <c r="E28" s="42">
-        <v>1</v>
-      </c>
-      <c r="F28" s="42"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="48"/>
-      <c r="J28" s="49"/>
-      <c r="K28" s="50"/>
-      <c r="L28" s="42"/>
-      <c r="M28" s="42">
-        <v>1</v>
-      </c>
-      <c r="N28" s="42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D29" s="44" t="s">
-        <v>61</v>
-      </c>
-      <c r="E29" s="42">
-        <v>1</v>
-      </c>
-      <c r="F29" s="42"/>
-      <c r="G29" s="43"/>
-      <c r="H29" s="43"/>
-      <c r="I29" s="48"/>
-      <c r="J29" s="49"/>
-      <c r="K29" s="50"/>
-      <c r="L29" s="42"/>
-      <c r="M29" s="42">
-        <v>1</v>
-      </c>
-      <c r="N29" s="42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D30" s="44" t="s">
-        <v>62</v>
-      </c>
-      <c r="E30" s="42">
-        <v>1</v>
-      </c>
-      <c r="F30" s="42"/>
-      <c r="G30" s="43"/>
-      <c r="H30" s="43"/>
-      <c r="I30" s="48"/>
-      <c r="J30" s="49"/>
-      <c r="K30" s="50"/>
-      <c r="L30" s="42"/>
-      <c r="M30" s="42">
-        <v>1</v>
-      </c>
-      <c r="N30" s="42">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="44">
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="I29:K29"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="I30:K30"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="I27:K27"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I28:K28"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="I25:K25"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="I21:K21"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="I17:K17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I12:K12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="I13:K13"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:K10"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>